<commit_message>
implimentation of path file
</commit_message>
<xml_diff>
--- a/src/test-data/data for sign-up chat.xlsx
+++ b/src/test-data/data for sign-up chat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Gyansetu\G_TestCase001\src\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497590C8-F54A-47E4-88D1-145918126D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7530C2-0D7C-4F26-B97A-F765E4BC72AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="1" r:id="rId1"/>
@@ -189,10 +189,10 @@
     <t>All is well</t>
   </si>
   <si>
-    <t>sarasu123@yopmail.com</t>
-  </si>
-  <si>
     <t>Sarasu VB</t>
+  </si>
+  <si>
+    <t>grukagriffere-8073@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -242,10 +242,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -594,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -618,10 +620,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B2" s="9">
-        <v>7675443123</v>
+        <v>7675443124</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>3</v>
@@ -671,8 +673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{592D667A-AC66-4967-A7EA-AD5EBA28D551}">
   <dimension ref="A1:AB7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -790,7 +792,7 @@
     </row>
     <row r="2" spans="1:28" ht="28.8">
       <c r="A2" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="5">
         <v>26</v>

</xml_diff>